<commit_message>
commit working round 3
</commit_message>
<xml_diff>
--- a/Disertation Bibliography .xlsx
+++ b/Disertation Bibliography .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camed\OneDrive\Documents\GitHub\Disertation_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3260C56E-F777-4C45-8E63-7A30D254A94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B885928-515E-4EC8-A9D7-CD2B2368045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="624" windowWidth="23040" windowHeight="11616" xr2:uid="{DA9A4906-27B9-443F-ABF8-51DF8D6D4076}"/>
+    <workbookView minimized="1" xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11235" xr2:uid="{DA9A4906-27B9-443F-ABF8-51DF8D6D4076}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
   <si>
     <t>Accessibility/usability</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>Codeless3D: Design and Usability Evaluation of a Low-Code Tool for 3D Game Generation | IEEE Journals &amp; Magazine | IEEE Xplore</t>
+  </si>
+  <si>
+    <t>http://gamma.cs.unc.edu/POWERPLANT/papers/ply.pdf</t>
   </si>
 </sst>
 </file>
@@ -909,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075AA31E-6108-44F3-8364-BAB4120DCED6}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1435,6 +1438,11 @@
       </c>
       <c r="C53" s="2" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="B54" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="26.25">

</xml_diff>